<commit_message>
- I had to reduce the array of hashes - sort the images hash because its order was messed up too - added new test case which tests the said order
</commit_message>
<xml_diff>
--- a/test/files/kangaroos.xlsx
+++ b/test/files/kangaroos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsushikanazawa/Projects/roo/test/image_order/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsushikanazawa/Projects/roo/test/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C656651-0F98-9448-8B66-DDA2027B88AA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEBB872-3384-1942-BD1C-173926F73AD9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{26305FCE-FEB1-4F40-A8B8-64E0329A93ED}"/>
+    <workbookView xWindow="8520" yWindow="3940" windowWidth="27640" windowHeight="16940" xr2:uid="{26305FCE-FEB1-4F40-A8B8-64E0329A93ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,6 +114,138 @@
         <a:xfrm>
           <a:off x="368300" y="317500"/>
           <a:ext cx="1905000" cy="1066800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{316865EE-66A7-AB43-9AC0-EB0A65FC0BF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="495300" y="1752600"/>
+          <a:ext cx="1739900" cy="1168400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{885933D3-1289-004D-ADC4-62A6D0ABDA49}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="558800" y="3352800"/>
+          <a:ext cx="1739900" cy="1155700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FAE5C9D-30D5-E84C-BDFA-34F976C34F17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="520700" y="5092700"/>
+          <a:ext cx="1752600" cy="1155700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -473,7 +605,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6E8A83-30CC-0D40-B8B5-408D3C71E06C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
@@ -498,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E772058-2A62-CD4A-9841-6631A4312F5C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>